<commit_message>
validar lista de producto en archivo datos particulares
Se agrego una condición  para validar que si el plan es A001, cambiar dos coberturas, porque la suma asegurada no puede estar en 0,

-En la data se actualizo,:
  -Registro uno planProd. A01 y forma de pago 12 meses.
  -Registros dos planProd. A002 y forma de pago Anual
</commit_message>
<xml_diff>
--- a/Components/DatosParticualres/Default.xlsx
+++ b/Components/DatosParticualres/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>USO_DEL_VEHICULO</t>
   </si>
@@ -29,6 +29,12 @@
     <t>BUSCAR_ZONA_GESTION</t>
   </si>
   <si>
+    <t>BUSCAR_LISTA_DE_COBERTURA</t>
+  </si>
+  <si>
+    <t>%A045</t>
+  </si>
+  <si>
     <t>P55RTA</t>
   </si>
   <si>
@@ -47,6 +53,9 @@
     <t>No Aplica</t>
   </si>
   <si>
+    <t>PLAN_DEL_PRODUCTO</t>
+  </si>
+  <si>
     <t>BMW</t>
   </si>
   <si>
@@ -89,6 +98,9 @@
     <t>ACUERDO_DE_PAGO</t>
   </si>
   <si>
+    <t>LISTA_DE_COBERTURA</t>
+  </si>
+  <si>
     <t>BUSCAR_LISTA_DE_TIPO</t>
   </si>
   <si>
@@ -107,6 +119,9 @@
     <t>LISTA_PAIS_ESTADO_PLACA</t>
   </si>
   <si>
+    <t>%A018</t>
+  </si>
+  <si>
     <t>LISTA_TIPO_MODELO</t>
   </si>
   <si>
@@ -119,6 +134,9 @@
     <t>%PUEBLA</t>
   </si>
   <si>
+    <t>BUSCAR_LISTA_DE_COBERTURA2</t>
+  </si>
+  <si>
     <t>AUTOMOVIL RESIDENTE</t>
   </si>
   <si>
@@ -171,6 +189,9 @@
   </si>
   <si>
     <t>TIPO_DE_REMOLQUE</t>
+  </si>
+  <si>
+    <t>AUTO INTEGRAL</t>
   </si>
 </sst>
 </file>
@@ -390,7 +411,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -690,194 +711,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="29" width="9.41796875" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="8.8984375" style="4" customWidth="1"/>
+    <col min="1" max="33" width="9.41796875" style="4" customWidth="1"/>
+    <col min="34" max="16384" width="8.8984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" s="9" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>2020</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2">
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="W2" s="6">
         <v>45391</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>